<commit_message>
add obs in some  tables
</commit_message>
<xml_diff>
--- a/result/t14/summary.xlsx
+++ b/result/t14/summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hirotake_ito/Documents/project/saitama2017/rae/result/t14/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s13592/Documents/project/other/rae/result/t14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA87DC3B-BF3F-9949-AAAC-8B9ACD367C3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD92C0D3-CABB-CE43-A780-BFACA1B5F0E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="20220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,20 @@
   <definedNames>
     <definedName name="memo" localSheetId="4">list!$A$1:$B$12</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -40,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5238" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5240" uniqueCount="351">
   <si>
     <t>name</t>
   </si>
@@ -1207,6 +1220,14 @@
     <t>\textbf{Parental characteristics}</t>
     <phoneticPr fontId="5"/>
   </si>
+  <si>
+    <t>obs</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Obs</t>
+    <phoneticPr fontId="5"/>
+  </si>
 </sst>
 </file>
 
@@ -1760,10 +1781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE47A3E-B22B-7440-808D-7BA82E16F6C8}">
-  <dimension ref="A2:Q66"/>
+  <dimension ref="A2:R66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="M3" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1776,14 +1797,15 @@
     <col min="8" max="9" width="17.5" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="10" max="10" width="10.83203125" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="11" max="12" width="14.1640625" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="14.1640625" style="3" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="24" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24" style="3" customWidth="1"/>
-    <col min="16" max="16" width="24" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="10.83203125" collapsed="1"/>
+    <col min="13" max="13" width="14.1640625" style="3" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="14" max="14" width="14.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="24" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24" style="3" customWidth="1"/>
+    <col min="17" max="17" width="24" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="10.83203125" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="18" collapsed="1">
+    <row r="2" spans="1:18" ht="18" collapsed="1">
       <c r="A2" s="8"/>
       <c r="C2" s="29"/>
       <c r="D2" s="12"/>
@@ -1799,8 +1821,9 @@
       <c r="N2" s="11"/>
       <c r="O2" s="11"/>
       <c r="P2" s="11"/>
-    </row>
-    <row r="3" spans="1:17" ht="19">
+      <c r="Q2" s="11"/>
+    </row>
+    <row r="3" spans="1:18" ht="19">
       <c r="A3" s="8"/>
       <c r="C3" s="30" t="s">
         <v>55</v>
@@ -1822,8 +1845,9 @@
       <c r="N3" s="20"/>
       <c r="O3" s="20"/>
       <c r="P3" s="20"/>
-    </row>
-    <row r="4" spans="1:17" ht="38">
+      <c r="Q3" s="20"/>
+    </row>
+    <row r="4" spans="1:18" ht="38">
       <c r="A4" s="8"/>
       <c r="B4" s="5"/>
       <c r="C4" s="29" t="s">
@@ -1845,19 +1869,22 @@
         <v>134</v>
       </c>
       <c r="M4" s="11" t="s">
+        <v>350</v>
+      </c>
+      <c r="N4" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="O4" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="P4" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="Q4" s="11" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="18" hidden="1" outlineLevel="1" collapsed="1">
+    <row r="5" spans="1:18" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A5" s="8"/>
       <c r="B5" s="15" t="s">
         <v>54</v>
@@ -1876,8 +1903,9 @@
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
-    </row>
-    <row r="6" spans="1:17" ht="18" hidden="1" outlineLevel="1">
+      <c r="Q5" s="7"/>
+    </row>
+    <row r="6" spans="1:18" ht="18" hidden="1" outlineLevel="1">
       <c r="A6" s="8"/>
       <c r="B6" s="5" t="s">
         <v>52</v>
@@ -1893,15 +1921,16 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
-      <c r="N6" s="5" t="s">
+      <c r="N6" s="5"/>
+      <c r="O6" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5" t="s">
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="18" hidden="1" outlineLevel="1">
+    <row r="7" spans="1:18" ht="18" hidden="1" outlineLevel="1">
       <c r="A7" s="8"/>
       <c r="B7" s="6"/>
       <c r="C7" s="32" t="s">
@@ -1919,15 +1948,16 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
-      <c r="N7" s="5" t="s">
+      <c r="N7" s="5"/>
+      <c r="O7" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5" t="s">
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="18" hidden="1" outlineLevel="1">
+    <row r="8" spans="1:18" ht="18" hidden="1" outlineLevel="1">
       <c r="A8" s="8"/>
       <c r="B8" s="6"/>
       <c r="C8" s="33" t="s">
@@ -1945,15 +1975,16 @@
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
       <c r="M8" s="14"/>
-      <c r="N8" s="14" t="s">
+      <c r="N8" s="14"/>
+      <c r="O8" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14" t="s">
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="18" hidden="1" outlineLevel="1">
+    <row r="9" spans="1:18" ht="18" hidden="1" outlineLevel="1">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="31"/>
@@ -1970,8 +2001,9 @@
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
-    </row>
-    <row r="10" spans="1:17" ht="18" hidden="1" outlineLevel="1">
+      <c r="Q9" s="9"/>
+    </row>
+    <row r="10" spans="1:18" ht="18" hidden="1" outlineLevel="1">
       <c r="A10" s="8"/>
       <c r="B10" s="6"/>
       <c r="C10" s="31"/>
@@ -1988,8 +2020,9 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
-    </row>
-    <row r="11" spans="1:17" ht="18" hidden="1" outlineLevel="1">
+      <c r="Q10" s="5"/>
+    </row>
+    <row r="11" spans="1:18" ht="18" hidden="1" outlineLevel="1">
       <c r="A11" s="8"/>
       <c r="B11" s="6"/>
       <c r="C11" s="31"/>
@@ -2006,11 +2039,12 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
-      <c r="Q11" t="s">
+      <c r="Q11" s="5"/>
+      <c r="R11" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="18" hidden="1" outlineLevel="1">
+    <row r="12" spans="1:18" ht="18" hidden="1" outlineLevel="1">
       <c r="A12" s="8"/>
       <c r="B12" s="6"/>
       <c r="C12" s="31"/>
@@ -2025,17 +2059,18 @@
       <c r="J12" s="6"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
-      <c r="N12" s="5" t="s">
-        <v>151</v>
-      </c>
+      <c r="M12" s="5"/>
       <c r="O12" s="5" t="s">
         <v>151</v>
       </c>
       <c r="P12" s="5" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" ht="18" hidden="1" outlineLevel="1">
+      <c r="Q12" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="18" hidden="1" outlineLevel="1">
       <c r="A13" s="8"/>
       <c r="B13" s="6"/>
       <c r="C13" s="31"/>
@@ -2051,17 +2086,18 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
-      <c r="N13" s="5" t="s">
-        <v>178</v>
-      </c>
+      <c r="N13" s="5"/>
       <c r="O13" s="5" t="s">
         <v>178</v>
       </c>
       <c r="P13" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q13" s="5" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="18" hidden="1" outlineLevel="1">
+    <row r="14" spans="1:18" ht="18" hidden="1" outlineLevel="1">
       <c r="A14" s="8"/>
       <c r="B14" s="6"/>
       <c r="C14" s="31"/>
@@ -2079,11 +2115,12 @@
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
-      <c r="P14" s="5" t="s">
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="18" hidden="1" outlineLevel="1">
+    <row r="15" spans="1:18" ht="18" hidden="1" outlineLevel="1">
       <c r="A15" s="8"/>
       <c r="B15" s="6"/>
       <c r="C15" s="31"/>
@@ -2100,8 +2137,9 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
-    </row>
-    <row r="16" spans="1:17" ht="18" hidden="1" outlineLevel="1">
+      <c r="Q15" s="5"/>
+    </row>
+    <row r="16" spans="1:18" ht="18" hidden="1" outlineLevel="1">
       <c r="A16" s="8"/>
       <c r="B16" s="6"/>
       <c r="C16" s="31"/>
@@ -2118,8 +2156,9 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
-    </row>
-    <row r="17" spans="1:16" ht="18" hidden="1" outlineLevel="1">
+      <c r="Q16" s="5"/>
+    </row>
+    <row r="17" spans="1:17" ht="18" hidden="1" outlineLevel="1">
       <c r="A17" s="8"/>
       <c r="B17" s="6"/>
       <c r="C17" s="31"/>
@@ -2136,8 +2175,9 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
-    </row>
-    <row r="18" spans="1:16" ht="18" hidden="1" outlineLevel="1">
+      <c r="Q17" s="5"/>
+    </row>
+    <row r="18" spans="1:17" ht="18" hidden="1" outlineLevel="1">
       <c r="A18" s="8"/>
       <c r="B18" s="5"/>
       <c r="C18" s="31"/>
@@ -2154,8 +2194,9 @@
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
-    </row>
-    <row r="19" spans="1:16" ht="18" hidden="1" outlineLevel="1">
+      <c r="Q18" s="5"/>
+    </row>
+    <row r="19" spans="1:17" ht="18" hidden="1" outlineLevel="1">
       <c r="A19" s="8"/>
       <c r="B19" s="5"/>
       <c r="C19" s="31"/>
@@ -2172,8 +2213,9 @@
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
-    </row>
-    <row r="20" spans="1:16" ht="18" hidden="1" outlineLevel="1">
+      <c r="Q19" s="5"/>
+    </row>
+    <row r="20" spans="1:17" ht="18" hidden="1" outlineLevel="1">
       <c r="A20" s="8"/>
       <c r="B20" s="5"/>
       <c r="C20" s="31"/>
@@ -2190,8 +2232,9 @@
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
-    </row>
-    <row r="21" spans="1:16" ht="18" collapsed="1">
+      <c r="Q20" s="5"/>
+    </row>
+    <row r="21" spans="1:17" ht="18" collapsed="1">
       <c r="A21" s="8"/>
       <c r="C21" s="34" t="s">
         <v>54</v>
@@ -2209,8 +2252,9 @@
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
       <c r="P21" s="7"/>
-    </row>
-    <row r="22" spans="1:16" ht="19">
+      <c r="Q21" s="7"/>
+    </row>
+    <row r="22" spans="1:17" ht="19">
       <c r="A22" s="8"/>
       <c r="C22" s="35" t="s">
         <v>348</v>
@@ -2228,8 +2272,9 @@
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
       <c r="P22" s="7"/>
-    </row>
-    <row r="23" spans="1:16" ht="38">
+      <c r="Q22" s="7"/>
+    </row>
+    <row r="23" spans="1:17" ht="38">
       <c r="A23" s="8"/>
       <c r="C23" s="31" t="str">
         <f>D23</f>
@@ -2260,24 +2305,28 @@
         <v>#REF!</v>
       </c>
       <c r="M23" s="7" t="str">
+        <f>INDEX(summary_glance!$AE:$AE,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H23),summary_glance!$Y:$Y,0),0)</f>
+        <v>569981</v>
+      </c>
+      <c r="N23" s="7" t="str">
         <f>TEXT(INDEX(summary_stat!$D:$D,MATCH(summary!F23,summary_stat!G:G,0),0)*G23,"0.000")</f>
         <v>29.941</v>
       </c>
-      <c r="N23" s="7" t="str">
-        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H23),summary_glance!$Y:$Y,0),0)</f>
+      <c r="O23" s="7" t="str">
+        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H23),summary_glance!$Y:$Y,0),0)</f>
         <v>-0.107
 (0.021)</v>
       </c>
-      <c r="O23" s="7" t="str">
-        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H23),summary_glance!$Y:$Y,0),0)</f>
-        <v>0.000</v>
-      </c>
-      <c r="P23" s="7" t="e">
-        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(P$12,"_",P$13,"_",$H23,"_",P$14),summary_tidy!$AA:$AA,0),0)</f>
+      <c r="P23" s="7" t="str">
+        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H23),summary_glance!$Y:$Y,0),0)</f>
+        <v>0.000</v>
+      </c>
+      <c r="Q23" s="7" t="e">
+        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(Q$12,"_",Q$13,"_",$H23,"_",Q$14),summary_tidy!$AA:$AA,0),0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="38">
+    <row r="24" spans="1:17" ht="38">
       <c r="A24" s="8"/>
       <c r="B24" s="7"/>
       <c r="C24" s="31" t="str">
@@ -2309,24 +2358,28 @@
         <v>#REF!</v>
       </c>
       <c r="M24" s="7" t="str">
+        <f>INDEX(summary_glance!$AE:$AE,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H24),summary_glance!$Y:$Y,0),0)</f>
+        <v>559098</v>
+      </c>
+      <c r="N24" s="7" t="str">
         <f>TEXT(INDEX(summary_stat!$D:$D,MATCH(summary!F24,summary_stat!G:G,0),0)*G24,"0.000")</f>
         <v>32.053</v>
       </c>
-      <c r="N24" s="7" t="str">
-        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H24),summary_glance!$Y:$Y,0),0)</f>
+      <c r="O24" s="7" t="str">
+        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H24),summary_glance!$Y:$Y,0),0)</f>
         <v>-0.125
 (0.023)</v>
       </c>
-      <c r="O24" s="7" t="str">
-        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H24),summary_glance!$Y:$Y,0),0)</f>
-        <v>0.000</v>
-      </c>
-      <c r="P24" s="7" t="e">
-        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(P$12,"_",P$13,"_",$H24,"_",P$14),summary_tidy!$AA:$AA,0),0)</f>
+      <c r="P24" s="7" t="str">
+        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H24),summary_glance!$Y:$Y,0),0)</f>
+        <v>0.000</v>
+      </c>
+      <c r="Q24" s="7" t="e">
+        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(Q$12,"_",Q$13,"_",$H24,"_",Q$14),summary_tidy!$AA:$AA,0),0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="38">
+    <row r="25" spans="1:17" ht="38">
       <c r="A25" s="8"/>
       <c r="B25" s="7"/>
       <c r="C25" s="29" t="str">
@@ -2358,24 +2411,28 @@
         <v>#REF!</v>
       </c>
       <c r="M25" s="11" t="str">
+        <f>INDEX(summary_glance!$AE:$AE,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H25),summary_glance!$Y:$Y,0),0)</f>
+        <v>569983</v>
+      </c>
+      <c r="N25" s="11" t="str">
         <f>TEXT(INDEX(summary_stat!$D:$D,MATCH(summary!F25,summary_stat!G:G,0),0)*G25,"0.000")</f>
         <v>1.910</v>
       </c>
-      <c r="N25" s="11" t="str">
-        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H25),summary_glance!$Y:$Y,0),0)</f>
+      <c r="O25" s="11" t="str">
+        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H25),summary_glance!$Y:$Y,0),0)</f>
         <v>-0.059
 (0.072)</v>
       </c>
-      <c r="O25" s="11" t="str">
-        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H25),summary_glance!$Y:$Y,0),0)</f>
+      <c r="P25" s="11" t="str">
+        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H25),summary_glance!$Y:$Y,0),0)</f>
         <v>0.561</v>
       </c>
-      <c r="P25" s="7" t="e">
-        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(P$12,"_",P$13,"_",$H25,"_",P$14),summary_tidy!$AA:$AA,0),0)</f>
+      <c r="Q25" s="7" t="e">
+        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(Q$12,"_",Q$13,"_",$H25,"_",Q$14),summary_tidy!$AA:$AA,0),0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="19" hidden="1" outlineLevel="1">
+    <row r="26" spans="1:17" ht="19" hidden="1" outlineLevel="1">
       <c r="A26" s="8"/>
       <c r="B26" s="7"/>
       <c r="C26" s="31" t="e">
@@ -2406,24 +2463,28 @@
         <f>INDEX(#REF!,MATCH(CONCATENATE($L$10,"_",$L$12,"_",$H26,"_within_grade"),#REF!, 0),0)</f>
         <v>#REF!</v>
       </c>
-      <c r="M26" s="7" t="str">
+      <c r="M26" s="7" t="e">
+        <f>INDEX(summary_glance!$AE:$AE,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H26),summary_glance!$Y:$Y,0),0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N26" s="7" t="str">
         <f>TEXT(INDEX(summary_stat!$D:$D,MATCH(summary!F26,summary_stat!G:G,0),0)*G26,"0.000")</f>
         <v>3.389</v>
       </c>
-      <c r="N26" s="7" t="e">
-        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H26),summary_glance!$Y:$Y,0),0)</f>
+      <c r="O26" s="7" t="e">
+        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H26),summary_glance!$Y:$Y,0),0)</f>
         <v>#N/A</v>
       </c>
-      <c r="O26" s="7" t="e">
-        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H26),summary_glance!$Y:$Y,0),0)</f>
+      <c r="P26" s="7" t="e">
+        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H26),summary_glance!$Y:$Y,0),0)</f>
         <v>#N/A</v>
       </c>
-      <c r="P26" s="7" t="e">
-        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(P$12,"_",P$13,"_",$H26,"_",P$14),summary_tidy!$AA:$AA,0),0)</f>
+      <c r="Q26" s="7" t="e">
+        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(Q$12,"_",Q$13,"_",$H26,"_",Q$14),summary_tidy!$AA:$AA,0),0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="38" hidden="1" outlineLevel="1">
+    <row r="27" spans="1:17" ht="38" hidden="1" outlineLevel="1">
       <c r="A27" s="8"/>
       <c r="B27" s="7"/>
       <c r="C27" s="29" t="str">
@@ -2454,24 +2515,28 @@
         <f>INDEX(#REF!,MATCH(CONCATENATE($L$10,"_",$L$12,"_",$H27,"_within_grade"),#REF!, 0),0)</f>
         <v>#REF!</v>
       </c>
-      <c r="M27" s="11" t="str">
+      <c r="M27" s="11" t="e">
+        <f>INDEX(summary_glance!$AE:$AE,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H27),summary_glance!$Y:$Y,0),0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N27" s="11" t="str">
         <f>TEXT(INDEX(summary_stat!$D:$D,MATCH(summary!F27,summary_stat!G:G,0),0)*G27,"0.000")</f>
         <v>41.608</v>
       </c>
-      <c r="N27" s="11" t="e">
-        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H27),summary_glance!$Y:$Y,0),0)</f>
+      <c r="O27" s="11" t="e">
+        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H27),summary_glance!$Y:$Y,0),0)</f>
         <v>#N/A</v>
       </c>
-      <c r="O27" s="11" t="e">
-        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H27),summary_glance!$Y:$Y,0),0)</f>
+      <c r="P27" s="11" t="e">
+        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H27),summary_glance!$Y:$Y,0),0)</f>
         <v>#N/A</v>
       </c>
-      <c r="P27" s="11" t="e">
-        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(P$12,"_",P$13,"_",$H27,"_",P$14),summary_tidy!$AA:$AA,0),0)</f>
+      <c r="Q27" s="11" t="e">
+        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(Q$12,"_",Q$13,"_",$H27,"_",Q$14),summary_tidy!$AA:$AA,0),0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="18" collapsed="1">
+    <row r="28" spans="1:17" ht="18" collapsed="1">
       <c r="A28" s="8"/>
       <c r="C28" s="36" t="s">
         <v>54</v>
@@ -2489,8 +2554,9 @@
       <c r="N28" s="7"/>
       <c r="O28" s="7"/>
       <c r="P28" s="7"/>
-    </row>
-    <row r="29" spans="1:16" ht="19">
+      <c r="Q28" s="7"/>
+    </row>
+    <row r="29" spans="1:17" ht="19">
       <c r="A29" s="8"/>
       <c r="C29" s="35" t="s">
         <v>347</v>
@@ -2508,8 +2574,9 @@
       <c r="N29" s="7"/>
       <c r="O29" s="7"/>
       <c r="P29" s="7"/>
-    </row>
-    <row r="30" spans="1:16" ht="38">
+      <c r="Q29" s="7"/>
+    </row>
+    <row r="30" spans="1:17" ht="38">
       <c r="A30" s="8"/>
       <c r="B30" s="7"/>
       <c r="C30" s="31" t="s">
@@ -2540,24 +2607,28 @@
         <v>#REF!</v>
       </c>
       <c r="M30" s="7" t="str">
+        <f>INDEX(summary_glance!$AE:$AE,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H30),summary_glance!$Y:$Y,0),0)</f>
+        <v>569983</v>
+      </c>
+      <c r="N30" s="7" t="str">
         <f>TEXT(INDEX(summary_stat!$D:$D,MATCH(summary!F30,summary_stat!G:G,0),0)*G30,"0.000")</f>
         <v>0.690</v>
       </c>
-      <c r="N30" s="7" t="str">
-        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H30),summary_glance!$Y:$Y,0),0)</f>
+      <c r="O30" s="7" t="str">
+        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H30),summary_glance!$Y:$Y,0),0)</f>
         <v>-0.002
 (0.039)</v>
       </c>
-      <c r="O30" s="7" t="str">
-        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H30),summary_glance!$Y:$Y,0),0)</f>
+      <c r="P30" s="7" t="str">
+        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H30),summary_glance!$Y:$Y,0),0)</f>
         <v>0.953</v>
       </c>
-      <c r="P30" s="7" t="e">
-        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(P$12,"_",P$13,"_",$H30,"_",P$14),summary_tidy!$AA:$AA,0),0)</f>
+      <c r="Q30" s="7" t="e">
+        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(Q$12,"_",Q$13,"_",$H30,"_",Q$14),summary_tidy!$AA:$AA,0),0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="38">
+    <row r="31" spans="1:17" ht="38">
       <c r="A31" s="8"/>
       <c r="B31" s="7"/>
       <c r="C31" s="31" t="s">
@@ -2588,24 +2659,28 @@
         <v>#REF!</v>
       </c>
       <c r="M31" s="7" t="str">
+        <f>INDEX(summary_glance!$AE:$AE,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H31),summary_glance!$Y:$Y,0),0)</f>
+        <v>569983</v>
+      </c>
+      <c r="N31" s="7" t="str">
         <f>TEXT(INDEX(summary_stat!$D:$D,MATCH(summary!F31,summary_stat!G:G,0),0)*G31,"0.000")</f>
         <v>7.185</v>
       </c>
-      <c r="N31" s="7" t="str">
-        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H31),summary_glance!$Y:$Y,0),0)</f>
+      <c r="O31" s="7" t="str">
+        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H31),summary_glance!$Y:$Y,0),0)</f>
         <v>-0.186
 (0.106)</v>
       </c>
-      <c r="O31" s="7" t="str">
-        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H31),summary_glance!$Y:$Y,0),0)</f>
+      <c r="P31" s="7" t="str">
+        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H31),summary_glance!$Y:$Y,0),0)</f>
         <v>0.199</v>
       </c>
-      <c r="P31" s="7" t="e">
-        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(P$12,"_",P$13,"_",$H31,"_",P$14),summary_tidy!$AA:$AA,0),0)</f>
+      <c r="Q31" s="7" t="e">
+        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(Q$12,"_",Q$13,"_",$H31,"_",Q$14),summary_tidy!$AA:$AA,0),0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="38">
+    <row r="32" spans="1:17" ht="38">
       <c r="A32" s="8"/>
       <c r="B32" s="7"/>
       <c r="C32" s="31" t="s">
@@ -2635,24 +2710,28 @@
         <v>#REF!</v>
       </c>
       <c r="M32" s="7" t="str">
+        <f>INDEX(summary_glance!$AE:$AE,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H32),summary_glance!$Y:$Y,0),0)</f>
+        <v>569983</v>
+      </c>
+      <c r="N32" s="7" t="str">
         <f>TEXT(INDEX(summary_stat!$D:$D,MATCH(summary!F32,summary_stat!G:G,0),0)*G32,"0.000")</f>
         <v>34.691</v>
       </c>
-      <c r="N32" s="7" t="str">
-        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H32),summary_glance!$Y:$Y,0),0)</f>
+      <c r="O32" s="7" t="str">
+        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H32),summary_glance!$Y:$Y,0),0)</f>
         <v>-0.033
 (0.238)</v>
       </c>
-      <c r="O32" s="7" t="str">
-        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H32),summary_glance!$Y:$Y,0),0)</f>
+      <c r="P32" s="7" t="str">
+        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H32),summary_glance!$Y:$Y,0),0)</f>
         <v>0.953</v>
       </c>
-      <c r="P32" s="7" t="e">
-        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(P$12,"_",P$13,"_",$H32,"_",P$14),summary_tidy!$AA:$AA,0),0)</f>
+      <c r="Q32" s="7" t="e">
+        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(Q$12,"_",Q$13,"_",$H32,"_",Q$14),summary_tidy!$AA:$AA,0),0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="38">
+    <row r="33" spans="1:17" ht="38">
       <c r="A33" s="8"/>
       <c r="B33" s="7"/>
       <c r="C33" s="31" t="s">
@@ -2683,24 +2762,28 @@
         <v>#REF!</v>
       </c>
       <c r="M33" s="7" t="str">
+        <f>INDEX(summary_glance!$AE:$AE,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H33),summary_glance!$Y:$Y,0),0)</f>
+        <v>569983</v>
+      </c>
+      <c r="N33" s="7" t="str">
         <f>TEXT(INDEX(summary_stat!$D:$D,MATCH(summary!F33,summary_stat!G:G,0),0)*G33,"0.000")</f>
         <v>41.608</v>
       </c>
-      <c r="N33" s="7" t="str">
-        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H33),summary_glance!$Y:$Y,0),0)</f>
+      <c r="O33" s="7" t="str">
+        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H33),summary_glance!$Y:$Y,0),0)</f>
         <v>-0.204
 (0.179)</v>
       </c>
-      <c r="O33" s="7" t="str">
-        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H33),summary_glance!$Y:$Y,0),0)</f>
+      <c r="P33" s="7" t="str">
+        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H33),summary_glance!$Y:$Y,0),0)</f>
         <v>0.425</v>
       </c>
-      <c r="P33" s="7" t="e">
-        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(P$12,"_",P$13,"_",$H33,"_",P$14),summary_tidy!$AA:$AA,0),0)</f>
+      <c r="Q33" s="7" t="e">
+        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(Q$12,"_",Q$13,"_",$H33,"_",Q$14),summary_tidy!$AA:$AA,0),0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="38">
+    <row r="34" spans="1:17" ht="38">
       <c r="A34" s="8"/>
       <c r="B34" s="7"/>
       <c r="C34" s="31" t="s">
@@ -2731,24 +2814,28 @@
         <v>#REF!</v>
       </c>
       <c r="M34" s="7" t="str">
+        <f>INDEX(summary_glance!$AE:$AE,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H34),summary_glance!$Y:$Y,0),0)</f>
+        <v>569983</v>
+      </c>
+      <c r="N34" s="7" t="str">
         <f>TEXT(INDEX(summary_stat!$D:$D,MATCH(summary!F34,summary_stat!G:G,0),0)*G34,"0.000")</f>
         <v>8.749</v>
       </c>
-      <c r="N34" s="7" t="str">
-        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H34),summary_glance!$Y:$Y,0),0)</f>
+      <c r="O34" s="7" t="str">
+        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H34),summary_glance!$Y:$Y,0),0)</f>
         <v>0.499
 (0.121)</v>
       </c>
-      <c r="O34" s="7" t="str">
-        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H34),summary_glance!$Y:$Y,0),0)</f>
-        <v>0.000</v>
-      </c>
-      <c r="P34" s="7" t="e">
-        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(P$12,"_",P$13,"_",$H34,"_",P$14),summary_tidy!$AA:$AA,0),0)</f>
+      <c r="P34" s="7" t="str">
+        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H34),summary_glance!$Y:$Y,0),0)</f>
+        <v>0.000</v>
+      </c>
+      <c r="Q34" s="7" t="e">
+        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(Q$12,"_",Q$13,"_",$H34,"_",Q$14),summary_tidy!$AA:$AA,0),0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="38">
+    <row r="35" spans="1:17" ht="38">
       <c r="A35" s="8"/>
       <c r="B35" s="7"/>
       <c r="C35" s="31" t="s">
@@ -2779,24 +2866,28 @@
         <v>#REF!</v>
       </c>
       <c r="M35" s="7" t="str">
+        <f>INDEX(summary_glance!$AE:$AE,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H35),summary_glance!$Y:$Y,0),0)</f>
+        <v>569983</v>
+      </c>
+      <c r="N35" s="7" t="str">
         <f>TEXT(INDEX(summary_stat!$D:$D,MATCH(summary!F35,summary_stat!G:G,0),0)*G35,"0.000")</f>
         <v>1.723</v>
       </c>
-      <c r="N35" s="7" t="str">
-        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H35),summary_glance!$Y:$Y,0),0)</f>
+      <c r="O35" s="7" t="str">
+        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H35),summary_glance!$Y:$Y,0),0)</f>
         <v>-0.155
 (0.050)</v>
       </c>
-      <c r="O35" s="7" t="str">
-        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H35),summary_glance!$Y:$Y,0),0)</f>
+      <c r="P35" s="7" t="str">
+        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H35),summary_glance!$Y:$Y,0),0)</f>
         <v>0.005</v>
       </c>
-      <c r="P35" s="7" t="e">
-        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(P$12,"_",P$13,"_",$H35,"_",P$14),summary_tidy!$AA:$AA,0),0)</f>
+      <c r="Q35" s="7" t="e">
+        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(Q$12,"_",Q$13,"_",$H35,"_",Q$14),summary_tidy!$AA:$AA,0),0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="38">
+    <row r="36" spans="1:17" ht="38">
       <c r="A36" s="8"/>
       <c r="B36" s="7"/>
       <c r="C36" s="29" t="s">
@@ -2827,24 +2918,28 @@
         <v>#REF!</v>
       </c>
       <c r="M36" s="11" t="str">
+        <f>INDEX(summary_glance!$AE:$AE,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H36),summary_glance!$Y:$Y,0),0)</f>
+        <v>569983</v>
+      </c>
+      <c r="N36" s="11" t="str">
         <f>TEXT(INDEX(summary_stat!$D:$D,MATCH(summary!F36,summary_stat!G:G,0),0)*G36,"0.000")</f>
         <v>5.354</v>
       </c>
-      <c r="N36" s="11" t="str">
-        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H36),summary_glance!$Y:$Y,0),0)</f>
+      <c r="O36" s="11" t="str">
+        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H36),summary_glance!$Y:$Y,0),0)</f>
         <v>0.081
 (0.192)</v>
       </c>
-      <c r="O36" s="11" t="str">
-        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H36),summary_glance!$Y:$Y,0),0)</f>
+      <c r="P36" s="11" t="str">
+        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H36),summary_glance!$Y:$Y,0),0)</f>
         <v>0.840</v>
       </c>
-      <c r="P36" s="7" t="e">
-        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(P$12,"_",P$13,"_",$H36,"_",P$14),summary_tidy!$AA:$AA,0),0)</f>
+      <c r="Q36" s="7" t="e">
+        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(Q$12,"_",Q$13,"_",$H36,"_",Q$14),summary_tidy!$AA:$AA,0),0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="18">
+    <row r="37" spans="1:17" ht="18">
       <c r="A37" s="8"/>
       <c r="C37" s="36" t="s">
         <v>54</v>
@@ -2862,8 +2957,9 @@
       <c r="N37" s="7"/>
       <c r="O37" s="7"/>
       <c r="P37" s="7"/>
-    </row>
-    <row r="38" spans="1:16" ht="19">
+      <c r="Q37" s="7"/>
+    </row>
+    <row r="38" spans="1:17" ht="19">
       <c r="A38" s="8"/>
       <c r="C38" s="35" t="s">
         <v>346</v>
@@ -2881,8 +2977,9 @@
       <c r="N38" s="7"/>
       <c r="O38" s="7"/>
       <c r="P38" s="7"/>
-    </row>
-    <row r="39" spans="1:16" ht="38">
+      <c r="Q38" s="7"/>
+    </row>
+    <row r="39" spans="1:17" ht="38">
       <c r="A39" s="8"/>
       <c r="B39" s="7"/>
       <c r="C39" s="31" t="str">
@@ -2914,24 +3011,28 @@
         <v>#REF!</v>
       </c>
       <c r="M39" s="7" t="str">
+        <f>INDEX(summary_glance!$AE:$AE,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H39),summary_glance!$Y:$Y,0),0)</f>
+        <v>569535</v>
+      </c>
+      <c r="N39" s="7" t="str">
         <f>TEXT(INDEX(summary_stat!$D:$D,MATCH(summary!F39,summary_stat!G:G,0),0)*G39,"0.000")</f>
         <v>3016.116</v>
       </c>
-      <c r="N39" s="7" t="str">
-        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H39),summary_glance!$Y:$Y,0),0)</f>
+      <c r="O39" s="7" t="str">
+        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H39),summary_glance!$Y:$Y,0),0)</f>
         <v>2.383
 (1.909)</v>
       </c>
-      <c r="O39" s="7" t="str">
-        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H39),summary_glance!$Y:$Y,0),0)</f>
+      <c r="P39" s="7" t="str">
+        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H39),summary_glance!$Y:$Y,0),0)</f>
         <v>0.398</v>
       </c>
-      <c r="P39" s="7" t="e">
-        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(P$12,"_",P$13,"_",$H39,"_",P$14),summary_tidy!$AA:$AA,0),0)</f>
+      <c r="Q39" s="7" t="e">
+        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(Q$12,"_",Q$13,"_",$H39,"_",Q$14),summary_tidy!$AA:$AA,0),0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="38">
+    <row r="40" spans="1:17" ht="38">
       <c r="A40" s="8"/>
       <c r="B40" s="7"/>
       <c r="C40" s="31" t="str">
@@ -2963,24 +3064,28 @@
         <v>#REF!</v>
       </c>
       <c r="M40" s="7" t="str">
+        <f>INDEX(summary_glance!$AE:$AE,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H40),summary_glance!$Y:$Y,0),0)</f>
+        <v>569784</v>
+      </c>
+      <c r="N40" s="7" t="str">
         <f>TEXT(INDEX(summary_stat!$D:$D,MATCH(summary!F40,summary_stat!G:G,0),0)*G40,"0.000")</f>
         <v>38.897</v>
       </c>
-      <c r="N40" s="7" t="str">
-        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H40),summary_glance!$Y:$Y,0),0)</f>
+      <c r="O40" s="7" t="str">
+        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H40),summary_glance!$Y:$Y,0),0)</f>
         <v>-0.002
 (0.009)</v>
       </c>
-      <c r="O40" s="7" t="str">
-        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H40),summary_glance!$Y:$Y,0),0)</f>
+      <c r="P40" s="7" t="str">
+        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H40),summary_glance!$Y:$Y,0),0)</f>
         <v>0.913</v>
       </c>
-      <c r="P40" s="7" t="e">
-        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(P$12,"_",P$13,"_",$H40,"_",P$14),summary_tidy!$AA:$AA,0),0)</f>
+      <c r="Q40" s="7" t="e">
+        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(Q$12,"_",Q$13,"_",$H40,"_",Q$14),summary_tidy!$AA:$AA,0),0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="38">
+    <row r="41" spans="1:17" ht="38">
       <c r="A41" s="8"/>
       <c r="B41" s="7"/>
       <c r="C41" s="31" t="str">
@@ -3011,24 +3116,28 @@
         <v>#REF!</v>
       </c>
       <c r="M41" s="7" t="str">
+        <f>INDEX(summary_glance!$AE:$AE,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H41),summary_glance!$Y:$Y,0),0)</f>
+        <v>569983</v>
+      </c>
+      <c r="N41" s="7" t="str">
         <f>TEXT(INDEX(summary_stat!$D:$D,MATCH(summary!F41,summary_stat!G:G,0),0)*G41,"0.000")</f>
         <v>97.951</v>
       </c>
-      <c r="N41" s="7" t="str">
-        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H41),summary_glance!$Y:$Y,0),0)</f>
+      <c r="O41" s="7" t="str">
+        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H41),summary_glance!$Y:$Y,0),0)</f>
         <v>-0.076
 (0.082)</v>
       </c>
-      <c r="O41" s="7" t="str">
-        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H41),summary_glance!$Y:$Y,0),0)</f>
+      <c r="P41" s="7" t="str">
+        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H41),summary_glance!$Y:$Y,0),0)</f>
         <v>0.528</v>
       </c>
-      <c r="P41" s="7" t="e">
-        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(P$12,"_",P$13,"_",$H41,"_",P$14),summary_tidy!$AA:$AA,0),0)</f>
+      <c r="Q41" s="7" t="e">
+        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(Q$12,"_",Q$13,"_",$H41,"_",Q$14),summary_tidy!$AA:$AA,0),0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="38">
+    <row r="42" spans="1:17" ht="38">
       <c r="A42" s="8"/>
       <c r="B42" s="7"/>
       <c r="C42" s="31" t="str">
@@ -3060,24 +3169,28 @@
         <v>#REF!</v>
       </c>
       <c r="M42" s="7" t="str">
+        <f>INDEX(summary_glance!$AE:$AE,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H42),summary_glance!$Y:$Y,0),0)</f>
+        <v>569983</v>
+      </c>
+      <c r="N42" s="7" t="str">
         <f>TEXT(INDEX(summary_stat!$D:$D,MATCH(summary!F42,summary_stat!G:G,0),0)*G42,"0.000")</f>
         <v>49.229</v>
       </c>
-      <c r="N42" s="7" t="str">
-        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H42),summary_glance!$Y:$Y,0),0)</f>
+      <c r="O42" s="7" t="str">
+        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H42),summary_glance!$Y:$Y,0),0)</f>
         <v>-1.007
 (0.259)</v>
       </c>
-      <c r="O42" s="7" t="str">
-        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H42),summary_glance!$Y:$Y,0),0)</f>
-        <v>0.000</v>
-      </c>
-      <c r="P42" s="7" t="e">
-        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(P$12,"_",P$13,"_",$H42,"_",P$14),summary_tidy!$AA:$AA,0),0)</f>
+      <c r="P42" s="7" t="str">
+        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H42),summary_glance!$Y:$Y,0),0)</f>
+        <v>0.000</v>
+      </c>
+      <c r="Q42" s="7" t="e">
+        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(Q$12,"_",Q$13,"_",$H42,"_",Q$14),summary_tidy!$AA:$AA,0),0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="38">
+    <row r="43" spans="1:17" ht="38">
       <c r="A43" s="8"/>
       <c r="B43" s="7"/>
       <c r="C43" s="29" t="str">
@@ -3109,24 +3222,28 @@
         <v>#REF!</v>
       </c>
       <c r="M43" s="11" t="str">
+        <f>INDEX(summary_glance!$AE:$AE,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H43),summary_glance!$Y:$Y,0),0)</f>
+        <v>569983</v>
+      </c>
+      <c r="N43" s="11" t="str">
         <f>TEXT(INDEX(summary_stat!$D:$D,MATCH(summary!F43,summary_stat!G:G,0),0)*G43,"0.000")</f>
         <v>48.710</v>
       </c>
-      <c r="N43" s="11" t="str">
-        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H43),summary_glance!$Y:$Y,0),0)</f>
+      <c r="O43" s="11" t="str">
+        <f>INDEX(summary_glance!$AD:$AD,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H43),summary_glance!$Y:$Y,0),0)</f>
         <v>-0.312
 (0.239)</v>
       </c>
-      <c r="O43" s="11" t="str">
-        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(N$12,"_",N$13,"_",$H43),summary_glance!$Y:$Y,0),0)</f>
+      <c r="P43" s="11" t="str">
+        <f>INDEX(summary_glance!$AC:$AC,MATCH(CONCATENATE(O$12,"_",O$13,"_",$H43),summary_glance!$Y:$Y,0),0)</f>
         <v>0.398</v>
       </c>
-      <c r="P43" s="11" t="e">
-        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(P$12,"_",P$13,"_",$H43,"_",P$14),summary_tidy!$AA:$AA,0),0)</f>
+      <c r="Q43" s="11" t="e">
+        <f>INDEX(summary_tidy!$AE:$AE,MATCH(CONCATENATE(Q$12,"_",Q$13,"_",$H43,"_",Q$14),summary_tidy!$AA:$AA,0),0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="18" hidden="1" outlineLevel="1">
+    <row r="44" spans="1:17" ht="18" hidden="1" outlineLevel="1">
       <c r="A44" s="8"/>
       <c r="B44" s="15" t="s">
         <v>54</v>
@@ -3145,8 +3262,9 @@
       <c r="N44" s="7"/>
       <c r="O44" s="7"/>
       <c r="P44" s="7"/>
-    </row>
-    <row r="45" spans="1:16" ht="19" hidden="1" outlineLevel="1">
+      <c r="Q44" s="7"/>
+    </row>
+    <row r="45" spans="1:17" ht="19" hidden="1" outlineLevel="1">
       <c r="A45" s="8"/>
       <c r="B45" s="7" t="s">
         <v>48</v>
@@ -3178,19 +3296,20 @@
         <v>#N/A</v>
       </c>
       <c r="M45" s="7"/>
-      <c r="N45" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(N$10,"_",$H45,N$12),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(N$10,"_",$H45,N$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="N45" s="7"/>
+      <c r="O45" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(O$10,"_",$H45,O$12),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(O$10,"_",$H45,O$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
-      <c r="O45" s="7"/>
-      <c r="P45" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(P$10,"_",$H45,P$12),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(P$10,"_",$H45,P$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="P45" s="7"/>
+      <c r="Q45" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(Q$10,"_",$H45,Q$12),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(Q$10,"_",$H45,Q$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="19" hidden="1" outlineLevel="1">
+    <row r="46" spans="1:17" ht="19" hidden="1" outlineLevel="1">
       <c r="A46" s="8"/>
       <c r="B46" s="7"/>
       <c r="C46" s="31" t="e">
@@ -3220,19 +3339,20 @@
         <v>#N/A</v>
       </c>
       <c r="M46" s="7"/>
-      <c r="N46" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(N$10,"_",$H46,N$12),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(N$10,"_",$H46,N$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="N46" s="7"/>
+      <c r="O46" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(O$10,"_",$H46,O$12),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(O$10,"_",$H46,O$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
-      <c r="O46" s="7"/>
-      <c r="P46" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(P$10,"_",$H46,P$12),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(P$10,"_",$H46,P$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="P46" s="7"/>
+      <c r="Q46" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(Q$10,"_",$H46,Q$12),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(Q$10,"_",$H46,Q$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="38" hidden="1" outlineLevel="1">
+    <row r="47" spans="1:17" ht="38" hidden="1" outlineLevel="1">
       <c r="A47" s="8"/>
       <c r="B47" s="7"/>
       <c r="C47" s="31" t="e">
@@ -3262,19 +3382,20 @@
         <v>#N/A</v>
       </c>
       <c r="M47" s="7"/>
-      <c r="N47" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(N$13,"_",$H47,N$15),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(N$13,"_",$H47,N$15),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="N47" s="7"/>
+      <c r="O47" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(O$13,"_",$H47,O$15),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(O$13,"_",$H47,O$15),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
-      <c r="O47" s="7"/>
-      <c r="P47" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(P$13,"_",$H47,P$15),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(P$13,"_",$H47,P$15),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="P47" s="7"/>
+      <c r="Q47" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(Q$13,"_",$H47,Q$15),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(Q$13,"_",$H47,Q$15),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="38" hidden="1" outlineLevel="1">
+    <row r="48" spans="1:17" ht="38" hidden="1" outlineLevel="1">
       <c r="A48" s="8"/>
       <c r="B48" s="7"/>
       <c r="C48" s="31" t="e">
@@ -3304,19 +3425,20 @@
         <v>#N/A</v>
       </c>
       <c r="M48" s="7"/>
-      <c r="N48" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(N$13,"_",$H48,N$15),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(N$13,"_",$H48,N$15),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="N48" s="7"/>
+      <c r="O48" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(O$13,"_",$H48,O$15),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(O$13,"_",$H48,O$15),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
-      <c r="O48" s="7"/>
-      <c r="P48" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(P$13,"_",$H48,P$15),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(P$13,"_",$H48,P$15),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="P48" s="7"/>
+      <c r="Q48" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(Q$13,"_",$H48,Q$15),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(Q$13,"_",$H48,Q$15),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="18" hidden="1" outlineLevel="1">
+    <row r="49" spans="1:17" ht="18" hidden="1" outlineLevel="1">
       <c r="A49" s="8"/>
       <c r="B49" s="15" t="s">
         <v>54</v>
@@ -3335,8 +3457,9 @@
       <c r="N49" s="7"/>
       <c r="O49" s="7"/>
       <c r="P49" s="7"/>
-    </row>
-    <row r="50" spans="1:16" ht="19" hidden="1" outlineLevel="1">
+      <c r="Q49" s="7"/>
+    </row>
+    <row r="50" spans="1:17" ht="19" hidden="1" outlineLevel="1">
       <c r="A50" s="8"/>
       <c r="B50" s="7" t="s">
         <v>49</v>
@@ -3368,19 +3491,20 @@
         <v>#N/A</v>
       </c>
       <c r="M50" s="7"/>
-      <c r="N50" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(N$10,"_",$H50,N$12),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(N$10,"_",$H50,N$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="N50" s="7"/>
+      <c r="O50" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(O$10,"_",$H50,O$12),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(O$10,"_",$H50,O$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
-      <c r="O50" s="7"/>
-      <c r="P50" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(P$10,"_",$H50,P$12),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(P$10,"_",$H50,P$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="P50" s="7"/>
+      <c r="Q50" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(Q$10,"_",$H50,Q$12),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(Q$10,"_",$H50,Q$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="38" hidden="1" outlineLevel="1">
+    <row r="51" spans="1:17" ht="38" hidden="1" outlineLevel="1">
       <c r="A51" s="8"/>
       <c r="B51" s="7"/>
       <c r="C51" s="31" t="e">
@@ -3410,19 +3534,20 @@
         <v>#N/A</v>
       </c>
       <c r="M51" s="7"/>
-      <c r="N51" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(N$13,"_",$H51,N$15),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(N$13,"_",$H51,N$15),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="N51" s="7"/>
+      <c r="O51" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(O$13,"_",$H51,O$15),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(O$13,"_",$H51,O$15),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
-      <c r="O51" s="7"/>
-      <c r="P51" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(P$13,"_",$H51,P$15),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(P$13,"_",$H51,P$15),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="P51" s="7"/>
+      <c r="Q51" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(Q$13,"_",$H51,Q$15),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(Q$13,"_",$H51,Q$15),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="38" hidden="1" outlineLevel="1">
+    <row r="52" spans="1:17" ht="38" hidden="1" outlineLevel="1">
       <c r="A52" s="8"/>
       <c r="B52" s="7"/>
       <c r="C52" s="29" t="e">
@@ -3452,24 +3577,25 @@
         <v>#N/A</v>
       </c>
       <c r="M52" s="11"/>
-      <c r="N52" s="11" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(N$13,"_",$H52,N$15),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(N$13,"_",$H52,N$15),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="N52" s="11"/>
+      <c r="O52" s="11" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(O$13,"_",$H52,O$15),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(O$13,"_",$H52,O$15),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
-      <c r="O52" s="11"/>
-      <c r="P52" s="11" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(P$13,"_",$H52,P$15),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(P$13,"_",$H52,P$15),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="P52" s="11"/>
+      <c r="Q52" s="11" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(Q$13,"_",$H52,Q$15),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(Q$13,"_",$H52,Q$15),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="53" spans="1:16" hidden="1" outlineLevel="1">
+    <row r="53" spans="1:17" hidden="1" outlineLevel="1">
       <c r="B53" s="15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="38" hidden="1" outlineLevel="1">
+    <row r="54" spans="1:17" ht="38" hidden="1" outlineLevel="1">
       <c r="A54" s="8"/>
       <c r="B54" s="7" t="s">
         <v>50</v>
@@ -3501,19 +3627,20 @@
         <v>#N/A</v>
       </c>
       <c r="M54" s="7"/>
-      <c r="N54" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(N$10,"_",$H54,N$12),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(N$10,"_",$H54,N$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="N54" s="7"/>
+      <c r="O54" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(O$10,"_",$H54,O$12),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(O$10,"_",$H54,O$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
-      <c r="O54" s="7"/>
-      <c r="P54" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(P$10,"_",$H54,P$12),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(P$10,"_",$H54,P$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="P54" s="7"/>
+      <c r="Q54" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(Q$10,"_",$H54,Q$12),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(Q$10,"_",$H54,Q$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="38" hidden="1" outlineLevel="1">
+    <row r="55" spans="1:17" ht="38" hidden="1" outlineLevel="1">
       <c r="A55" s="8"/>
       <c r="B55" s="7"/>
       <c r="C55" s="31" t="e">
@@ -3543,19 +3670,20 @@
         <v>#N/A</v>
       </c>
       <c r="M55" s="7"/>
-      <c r="N55" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(N$10,"_",$H55,N$12),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(N$10,"_",$H55,N$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="N55" s="7"/>
+      <c r="O55" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(O$10,"_",$H55,O$12),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(O$10,"_",$H55,O$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
-      <c r="O55" s="7"/>
-      <c r="P55" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(P$10,"_",$H55,P$12),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(P$10,"_",$H55,P$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="P55" s="7"/>
+      <c r="Q55" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(Q$10,"_",$H55,Q$12),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(Q$10,"_",$H55,Q$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="22" customFormat="1" ht="19" hidden="1" outlineLevel="1">
+    <row r="56" spans="1:17" s="22" customFormat="1" ht="19" hidden="1" outlineLevel="1">
       <c r="A56" s="21"/>
       <c r="B56" s="7"/>
       <c r="C56" s="31" t="e">
@@ -3585,19 +3713,20 @@
         <v>#N/A</v>
       </c>
       <c r="M56" s="7"/>
-      <c r="N56" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(N$10,"_",$H56,N$12),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(N$10,"_",$H56,N$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="N56" s="7"/>
+      <c r="O56" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(O$10,"_",$H56,O$12),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(O$10,"_",$H56,O$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
-      <c r="O56" s="7"/>
-      <c r="P56" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(P$10,"_",$H56,P$12),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(P$10,"_",$H56,P$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="P56" s="7"/>
+      <c r="Q56" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(Q$10,"_",$H56,Q$12),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(Q$10,"_",$H56,Q$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="38" hidden="1" outlineLevel="1">
+    <row r="57" spans="1:17" ht="38" hidden="1" outlineLevel="1">
       <c r="A57" s="8"/>
       <c r="B57" s="7"/>
       <c r="C57" s="31" t="e">
@@ -3627,19 +3756,20 @@
         <v>#N/A</v>
       </c>
       <c r="M57" s="7"/>
-      <c r="N57" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(N$10,"_",$H57,N$12),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(N$10,"_",$H57,N$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="N57" s="7"/>
+      <c r="O57" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(O$10,"_",$H57,O$12),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(O$10,"_",$H57,O$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
-      <c r="O57" s="7"/>
-      <c r="P57" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(P$10,"_",$H57,P$12),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(P$10,"_",$H57,P$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="P57" s="7"/>
+      <c r="Q57" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(Q$10,"_",$H57,Q$12),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(Q$10,"_",$H57,Q$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="38" hidden="1" outlineLevel="1">
+    <row r="58" spans="1:17" ht="38" hidden="1" outlineLevel="1">
       <c r="A58" s="8"/>
       <c r="B58" s="7"/>
       <c r="C58" s="29" t="e">
@@ -3669,24 +3799,25 @@
         <v>#N/A</v>
       </c>
       <c r="M58" s="11"/>
-      <c r="N58" s="11" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(N$10,"_",$H58,N$12),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(N$10,"_",$H58,N$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="N58" s="11"/>
+      <c r="O58" s="11" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(O$10,"_",$H58,O$12),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(O$10,"_",$H58,O$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
-      <c r="O58" s="11"/>
-      <c r="P58" s="11" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(P$10,"_",$H58,P$12),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(P$10,"_",$H58,P$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="P58" s="11"/>
+      <c r="Q58" s="11" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(Q$10,"_",$H58,Q$12),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(Q$10,"_",$H58,Q$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="59" spans="1:16" hidden="1" outlineLevel="1">
+    <row r="59" spans="1:17" hidden="1" outlineLevel="1">
       <c r="B59" s="15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="38" hidden="1" outlineLevel="1">
+    <row r="60" spans="1:17" ht="38" hidden="1" outlineLevel="1">
       <c r="A60" s="8"/>
       <c r="B60" s="7" t="s">
         <v>51</v>
@@ -3718,19 +3849,20 @@
         <v>#N/A</v>
       </c>
       <c r="M60" s="7"/>
-      <c r="N60" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(N$10,"_",$H60,N$12),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(N$10,"_",$H60,N$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="N60" s="7"/>
+      <c r="O60" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(O$10,"_",$H60,O$12),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(O$10,"_",$H60,O$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
-      <c r="O60" s="7"/>
-      <c r="P60" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(P$10,"_",$H60,P$12),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(P$10,"_",$H60,P$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="P60" s="7"/>
+      <c r="Q60" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(Q$10,"_",$H60,Q$12),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(Q$10,"_",$H60,Q$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="38" hidden="1" outlineLevel="1">
+    <row r="61" spans="1:17" ht="38" hidden="1" outlineLevel="1">
       <c r="A61" s="8"/>
       <c r="B61" s="7"/>
       <c r="C61" s="31" t="e">
@@ -3760,19 +3892,20 @@
         <v>#N/A</v>
       </c>
       <c r="M61" s="7"/>
-      <c r="N61" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(N$10,"_",$H61,N$12),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(N$10,"_",$H61,N$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="N61" s="7"/>
+      <c r="O61" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(O$10,"_",$H61,O$12),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(O$10,"_",$H61,O$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
-      <c r="O61" s="7"/>
-      <c r="P61" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(P$10,"_",$H61,P$12),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(P$10,"_",$H61,P$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="P61" s="7"/>
+      <c r="Q61" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(Q$10,"_",$H61,Q$12),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(Q$10,"_",$H61,Q$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="19" hidden="1" outlineLevel="1">
+    <row r="62" spans="1:17" ht="19" hidden="1" outlineLevel="1">
       <c r="A62" s="8"/>
       <c r="B62" s="7"/>
       <c r="C62" s="31" t="e">
@@ -3802,19 +3935,20 @@
         <v>#N/A</v>
       </c>
       <c r="M62" s="7"/>
-      <c r="N62" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(N$10,"_",$H62,N$12),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(N$10,"_",$H62,N$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="N62" s="7"/>
+      <c r="O62" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(O$10,"_",$H62,O$12),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(O$10,"_",$H62,O$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
-      <c r="O62" s="7"/>
-      <c r="P62" s="7" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(P$10,"_",$H62,P$12),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(P$10,"_",$H62,P$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="P62" s="7"/>
+      <c r="Q62" s="7" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(Q$10,"_",$H62,Q$12),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(Q$10,"_",$H62,Q$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="38" hidden="1" outlineLevel="1">
+    <row r="63" spans="1:17" ht="38" hidden="1" outlineLevel="1">
       <c r="A63" s="8"/>
       <c r="B63" s="7"/>
       <c r="C63" s="29" t="e">
@@ -3844,19 +3978,20 @@
         <v>#N/A</v>
       </c>
       <c r="M63" s="11"/>
-      <c r="N63" s="11" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(N$10,"_",$H63,N$12),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(N$10,"_",$H63,N$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="N63" s="11"/>
+      <c r="O63" s="11" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(O$10,"_",$H63,O$12),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(O$10,"_",$H63,O$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
-      <c r="O63" s="11"/>
-      <c r="P63" s="11" t="e">
-        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(P$10,"_",$H63,P$12),summary_glance!$Y:$Y,0),0)&amp;"
-("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(P$10,"_",$H63,P$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
+      <c r="P63" s="11"/>
+      <c r="Q63" s="11" t="e">
+        <f>INDEX(summary_glance!$AA:$AA,MATCH(CONCATENATE(Q$10,"_",$H63,Q$12),summary_glance!$Y:$Y,0),0)&amp;"
+("&amp;INDEX(summary_glance!$AB:$AB,MATCH(CONCATENATE(Q$10,"_",$H63,Q$12),summary_glance!$Y:$Y,0),0)&amp;")"</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="64" spans="1:16" collapsed="1">
+    <row r="64" spans="1:17" collapsed="1">
       <c r="C64" s="30" t="s">
         <v>54</v>
       </c>
@@ -3873,8 +4008,9 @@
       <c r="N64" s="27"/>
       <c r="O64" s="27"/>
       <c r="P64" s="27"/>
-    </row>
-    <row r="65" spans="1:16" ht="18">
+      <c r="Q64" s="27"/>
+    </row>
+    <row r="65" spans="1:17" ht="18">
       <c r="A65" s="8"/>
       <c r="B65" s="7"/>
       <c r="C65" s="29" t="s">
@@ -3889,14 +4025,15 @@
       <c r="J65" s="11"/>
       <c r="K65" s="11"/>
       <c r="L65" s="11"/>
-      <c r="M65" s="11">
+      <c r="M65" s="11"/>
+      <c r="N65" s="11">
         <v>569983</v>
       </c>
-      <c r="N65" s="11"/>
       <c r="O65" s="11"/>
       <c r="P65" s="11"/>
-    </row>
-    <row r="66" spans="1:16">
+      <c r="Q65" s="11"/>
+    </row>
+    <row r="66" spans="1:17">
       <c r="C66" s="34" t="s">
         <v>55</v>
       </c>
@@ -3909,10 +4046,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD121"/>
+  <dimension ref="A1:AE121"/>
   <sheetViews>
-    <sheetView zoomScale="65" workbookViewId="0">
-      <selection sqref="A1:S1048576"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AE77" sqref="AE2:AE77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -3922,7 +4059,7 @@
     <col min="25" max="25" width="40.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:31">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3996,8 +4133,11 @@
       <c r="AD1" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="2" spans="1:30">
+      <c r="AE1" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4082,8 +4222,12 @@
         <v>-0.125
 (0.023)</v>
       </c>
-    </row>
-    <row r="3" spans="1:30">
+      <c r="AE2" t="str">
+        <f>TEXT(I2,"0")</f>
+        <v>559098</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -4168,8 +4312,12 @@
         <v>-0.126
 (0.025)</v>
       </c>
-    </row>
-    <row r="4" spans="1:30">
+      <c r="AE3" t="str">
+        <f t="shared" ref="AE3:AE66" si="6">TEXT(I3,"0")</f>
+        <v>559098</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -4253,8 +4401,12 @@
         <v>-0.129
 (0.025)</v>
       </c>
-    </row>
-    <row r="5" spans="1:30">
+      <c r="AE4" t="str">
+        <f t="shared" si="6"/>
+        <v>559098</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4338,8 +4490,12 @@
         <v>-0.107
 (0.021)</v>
       </c>
-    </row>
-    <row r="6" spans="1:30">
+      <c r="AE5" t="str">
+        <f t="shared" si="6"/>
+        <v>569981</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4423,8 +4579,12 @@
         <v>-0.109
 (0.021)</v>
       </c>
-    </row>
-    <row r="7" spans="1:30">
+      <c r="AE6" t="str">
+        <f t="shared" si="6"/>
+        <v>569981</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4508,8 +4668,12 @@
         <v>-0.114
 (0.021)</v>
       </c>
-    </row>
-    <row r="8" spans="1:30">
+      <c r="AE7" t="str">
+        <f t="shared" si="6"/>
+        <v>569981</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4593,8 +4757,12 @@
         <v>-0.059
 (0.072)</v>
       </c>
-    </row>
-    <row r="9" spans="1:30">
+      <c r="AE8" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -4678,8 +4846,12 @@
         <v>-0.065
 (0.060)</v>
       </c>
-    </row>
-    <row r="10" spans="1:30">
+      <c r="AE9" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4763,8 +4935,12 @@
         <v>-0.062
 (0.060)</v>
       </c>
-    </row>
-    <row r="11" spans="1:30">
+      <c r="AE10" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4848,8 +5024,12 @@
         <v>2.383
 (1.909)</v>
       </c>
-    </row>
-    <row r="12" spans="1:30">
+      <c r="AE11" t="str">
+        <f t="shared" si="6"/>
+        <v>569535</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -4933,8 +5113,12 @@
         <v>2.602
 (1.928)</v>
       </c>
-    </row>
-    <row r="13" spans="1:30">
+      <c r="AE12" t="str">
+        <f t="shared" si="6"/>
+        <v>569535</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -5018,8 +5202,12 @@
         <v>2.588
 (1.926)</v>
       </c>
-    </row>
-    <row r="14" spans="1:30">
+      <c r="AE13" t="str">
+        <f t="shared" si="6"/>
+        <v>569535</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -5103,8 +5291,12 @@
         <v>-0.002
 (0.009)</v>
       </c>
-    </row>
-    <row r="15" spans="1:30">
+      <c r="AE14" t="str">
+        <f t="shared" si="6"/>
+        <v>569784</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -5188,8 +5380,12 @@
         <v>-0.003
 (0.012)</v>
       </c>
-    </row>
-    <row r="16" spans="1:30">
+      <c r="AE15" t="str">
+        <f t="shared" si="6"/>
+        <v>569784</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -5273,8 +5469,12 @@
         <v>-0.002
 (0.012)</v>
       </c>
-    </row>
-    <row r="17" spans="1:30">
+      <c r="AE16" t="str">
+        <f t="shared" si="6"/>
+        <v>569784</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -5358,8 +5558,12 @@
         <v>-0.076
 (0.082)</v>
       </c>
-    </row>
-    <row r="18" spans="1:30">
+      <c r="AE17" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -5443,8 +5647,12 @@
         <v>-0.080
 (0.062)</v>
       </c>
-    </row>
-    <row r="19" spans="1:30">
+      <c r="AE18" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -5528,8 +5736,12 @@
         <v>-0.080
 (0.062)</v>
       </c>
-    </row>
-    <row r="20" spans="1:30">
+      <c r="AE19" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -5613,8 +5825,12 @@
         <v>-1.007
 (0.259)</v>
       </c>
-    </row>
-    <row r="21" spans="1:30">
+      <c r="AE20" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -5698,8 +5914,12 @@
         <v>-1.023
 (0.220)</v>
       </c>
-    </row>
-    <row r="22" spans="1:30">
+      <c r="AE21" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -5783,8 +6003,12 @@
         <v>-0.992
 (0.220)</v>
       </c>
-    </row>
-    <row r="23" spans="1:30">
+      <c r="AE22" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -5868,8 +6092,12 @@
         <v>-0.312
 (0.239)</v>
       </c>
-    </row>
-    <row r="24" spans="1:30">
+      <c r="AE23" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -5953,8 +6181,12 @@
         <v>-0.316
 (0.220)</v>
       </c>
-    </row>
-    <row r="25" spans="1:30">
+      <c r="AE24" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -6038,8 +6270,12 @@
         <v>-0.329
 (0.220)</v>
       </c>
-    </row>
-    <row r="26" spans="1:30">
+      <c r="AE25" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -6099,33 +6335,37 @@
       </c>
       <c r="T26" s="1"/>
       <c r="Y26" s="1" t="str">
-        <f t="shared" ref="Y26:Y49" si="6">N26</f>
+        <f t="shared" ref="Y26:Y49" si="7">N26</f>
         <v>all_ols_I(job1*100)</v>
       </c>
       <c r="Z26" s="1">
-        <f t="shared" ref="Z26:Z49" si="7">ROUND(I26, 3)</f>
+        <f t="shared" ref="Z26:Z49" si="8">ROUND(I26, 3)</f>
         <v>569983</v>
       </c>
       <c r="AA26" s="1" t="str">
-        <f t="shared" ref="AA26:AA49" si="8">TEXT(K26,"0.000")</f>
+        <f t="shared" ref="AA26:AA49" si="9">TEXT(K26,"0.000")</f>
         <v>-0.002</v>
       </c>
       <c r="AB26" s="1" t="str">
-        <f t="shared" ref="AB26:AB49" si="9">TEXT(L26,"0.000")</f>
+        <f t="shared" ref="AB26:AB49" si="10">TEXT(L26,"0.000")</f>
         <v>0.039</v>
       </c>
       <c r="AC26" s="1" t="str">
-        <f t="shared" ref="AC26:AC49" si="10">TEXT(R26,"0.000")</f>
+        <f t="shared" ref="AC26:AC49" si="11">TEXT(R26,"0.000")</f>
         <v>0.953</v>
       </c>
       <c r="AD26" t="str">
-        <f t="shared" ref="AD26:AD49" si="11">CONCATENATE(AA26,"
+        <f t="shared" ref="AD26:AD49" si="12">CONCATENATE(AA26,"
 (",AB26,")")</f>
         <v>-0.002
 (0.039)</v>
       </c>
-    </row>
-    <row r="27" spans="1:30">
+      <c r="AE26" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -6185,32 +6425,36 @@
       </c>
       <c r="T27" s="1"/>
       <c r="Y27" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>all_no_live_I(job1*100)</v>
       </c>
       <c r="Z27" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>569983</v>
       </c>
       <c r="AA27" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.014</v>
       </c>
       <c r="AB27" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.036</v>
       </c>
       <c r="AC27" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.803</v>
       </c>
       <c r="AD27" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.014
 (0.036)</v>
       </c>
-    </row>
-    <row r="28" spans="1:30">
+      <c r="AE27" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -6270,32 +6514,36 @@
       </c>
       <c r="T28" s="1"/>
       <c r="Y28" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>all_no_live_liner_I(job1*100)</v>
       </c>
       <c r="Z28" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>569983</v>
       </c>
       <c r="AA28" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.016</v>
       </c>
       <c r="AB28" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.036</v>
       </c>
       <c r="AC28" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.756</v>
       </c>
       <c r="AD28" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.016
 (0.036)</v>
       </c>
-    </row>
-    <row r="29" spans="1:30">
+      <c r="AE28" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -6355,32 +6603,36 @@
       </c>
       <c r="T29" s="1"/>
       <c r="Y29" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>all_ols_I(job2*100)</v>
       </c>
       <c r="Z29" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>569983</v>
       </c>
       <c r="AA29" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.186</v>
       </c>
       <c r="AB29" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.106</v>
       </c>
       <c r="AC29" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.199</v>
       </c>
       <c r="AD29" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.186
 (0.106)</v>
       </c>
-    </row>
-    <row r="30" spans="1:30">
+      <c r="AE29" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -6440,32 +6692,36 @@
       </c>
       <c r="T30" s="1"/>
       <c r="Y30" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>all_no_live_I(job2*100)</v>
       </c>
       <c r="Z30" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>569983</v>
       </c>
       <c r="AA30" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.166</v>
       </c>
       <c r="AB30" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.114</v>
       </c>
       <c r="AC30" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.324</v>
       </c>
       <c r="AD30" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.166
 (0.114)</v>
       </c>
-    </row>
-    <row r="31" spans="1:30">
+      <c r="AE30" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -6524,32 +6780,36 @@
         <v>15</v>
       </c>
       <c r="Y31" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>all_no_live_liner_I(job2*100)</v>
       </c>
       <c r="Z31" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>569983</v>
       </c>
       <c r="AA31" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.156</v>
       </c>
       <c r="AB31" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.114</v>
       </c>
       <c r="AC31" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.333</v>
       </c>
       <c r="AD31" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.156
 (0.114)</v>
       </c>
-    </row>
-    <row r="32" spans="1:30">
+      <c r="AE31" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -6608,32 +6868,36 @@
         <v>15</v>
       </c>
       <c r="Y32" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>all_ols_I(job3*100)</v>
       </c>
       <c r="Z32" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>569983</v>
       </c>
       <c r="AA32" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.033</v>
       </c>
       <c r="AB32" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.238</v>
       </c>
       <c r="AC32" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.953</v>
       </c>
       <c r="AD32" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.033
 (0.238)</v>
       </c>
-    </row>
-    <row r="33" spans="1:30">
+      <c r="AE32" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -6692,32 +6956,36 @@
         <v>15</v>
       </c>
       <c r="Y33" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>all_no_live_I(job3*100)</v>
       </c>
       <c r="Z33" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>569983</v>
       </c>
       <c r="AA33" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.040</v>
       </c>
       <c r="AB33" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.210</v>
       </c>
       <c r="AC33" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.850</v>
       </c>
       <c r="AD33" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.040
 (0.210)</v>
       </c>
-    </row>
-    <row r="34" spans="1:30">
+      <c r="AE33" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -6776,32 +7044,36 @@
         <v>15</v>
       </c>
       <c r="Y34" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>all_no_live_liner_I(job3*100)</v>
       </c>
       <c r="Z34" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>569983</v>
       </c>
       <c r="AA34" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.063</v>
       </c>
       <c r="AB34" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.210</v>
       </c>
       <c r="AC34" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.819</v>
       </c>
       <c r="AD34" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.063
 (0.210)</v>
       </c>
-    </row>
-    <row r="35" spans="1:30">
+      <c r="AE34" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="35" spans="1:31">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -6860,32 +7132,36 @@
         <v>15</v>
       </c>
       <c r="Y35" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>all_ols_I(job4*100)</v>
       </c>
       <c r="Z35" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>569983</v>
       </c>
       <c r="AA35" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.204</v>
       </c>
       <c r="AB35" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.179</v>
       </c>
       <c r="AC35" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.425</v>
       </c>
       <c r="AD35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.204
 (0.179)</v>
       </c>
-    </row>
-    <row r="36" spans="1:30">
+      <c r="AE35" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -6944,32 +7220,36 @@
         <v>15</v>
       </c>
       <c r="Y36" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>all_no_live_I(job4*100)</v>
       </c>
       <c r="Z36" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>569983</v>
       </c>
       <c r="AA36" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.253</v>
       </c>
       <c r="AB36" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.217</v>
       </c>
       <c r="AC36" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.348</v>
       </c>
       <c r="AD36" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.253
 (0.217)</v>
       </c>
-    </row>
-    <row r="37" spans="1:30">
+      <c r="AE36" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -7028,32 +7308,36 @@
         <v>15</v>
       </c>
       <c r="Y37" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>all_no_live_liner_I(job4*100)</v>
       </c>
       <c r="Z37" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>569983</v>
       </c>
       <c r="AA37" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.258</v>
       </c>
       <c r="AB37" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.217</v>
       </c>
       <c r="AC37" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.352</v>
       </c>
       <c r="AD37" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.258
 (0.217)</v>
       </c>
-    </row>
-    <row r="38" spans="1:30">
+      <c r="AE37" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -7112,32 +7396,36 @@
         <v>15</v>
       </c>
       <c r="Y38" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>all_ols_I(job5*100)</v>
       </c>
       <c r="Z38" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>569983</v>
       </c>
       <c r="AA38" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.499</v>
       </c>
       <c r="AB38" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.121</v>
       </c>
       <c r="AC38" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.000</v>
       </c>
       <c r="AD38" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.499
 (0.121)</v>
       </c>
-    </row>
-    <row r="39" spans="1:30">
+      <c r="AE38" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -7196,32 +7484,36 @@
         <v>15</v>
       </c>
       <c r="Y39" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>all_no_live_I(job5*100)</v>
       </c>
       <c r="Z39" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>569983</v>
       </c>
       <c r="AA39" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.490</v>
       </c>
       <c r="AB39" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.125</v>
       </c>
       <c r="AC39" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.000</v>
       </c>
       <c r="AD39" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.490
 (0.125)</v>
       </c>
-    </row>
-    <row r="40" spans="1:30">
+      <c r="AE39" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="40" spans="1:31">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -7280,32 +7572,36 @@
         <v>15</v>
       </c>
       <c r="Y40" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>all_no_live_liner_I(job5*100)</v>
       </c>
       <c r="Z40" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>569983</v>
       </c>
       <c r="AA40" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.498</v>
       </c>
       <c r="AB40" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.124</v>
       </c>
       <c r="AC40" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.000</v>
       </c>
       <c r="AD40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.498
 (0.124)</v>
       </c>
-    </row>
-    <row r="41" spans="1:30">
+      <c r="AE40" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -7364,32 +7660,36 @@
         <v>15</v>
       </c>
       <c r="Y41" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>all_ols_I(job6*100)</v>
       </c>
       <c r="Z41" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>569983</v>
       </c>
       <c r="AA41" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.155</v>
       </c>
       <c r="AB41" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.050</v>
       </c>
       <c r="AC41" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.005</v>
       </c>
       <c r="AD41" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.155
 (0.050)</v>
       </c>
-    </row>
-    <row r="42" spans="1:30">
+      <c r="AE41" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -7448,32 +7748,36 @@
         <v>15</v>
       </c>
       <c r="Y42" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>all_no_live_I(job6*100)</v>
       </c>
       <c r="Z42" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>569983</v>
       </c>
       <c r="AA42" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.156</v>
       </c>
       <c r="AB42" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.057</v>
       </c>
       <c r="AC42" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.020</v>
       </c>
       <c r="AD42" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.156
 (0.057)</v>
       </c>
-    </row>
-    <row r="43" spans="1:30">
+      <c r="AE42" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -7532,32 +7836,36 @@
         <v>15</v>
       </c>
       <c r="Y43" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>all_no_live_liner_I(job6*100)</v>
       </c>
       <c r="Z43" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>569983</v>
       </c>
       <c r="AA43" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.148</v>
       </c>
       <c r="AB43" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.057</v>
       </c>
       <c r="AC43" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.029</v>
       </c>
       <c r="AD43" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.148
 (0.057)</v>
       </c>
-    </row>
-    <row r="44" spans="1:30">
+      <c r="AE43" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -7616,32 +7924,36 @@
         <v>15</v>
       </c>
       <c r="Y44" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>all_ols_I(job7V*100)</v>
       </c>
       <c r="Z44" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>569983</v>
       </c>
       <c r="AA44" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.081</v>
       </c>
       <c r="AB44" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.192</v>
       </c>
       <c r="AC44" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.840</v>
       </c>
       <c r="AD44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.081
 (0.192)</v>
       </c>
-    </row>
-    <row r="45" spans="1:30">
+      <c r="AE44" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -7700,32 +8012,36 @@
         <v>15</v>
       </c>
       <c r="Y45" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>all_no_live_I(job7V*100)</v>
       </c>
       <c r="Z45" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>569983</v>
       </c>
       <c r="AA45" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.110</v>
       </c>
       <c r="AB45" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.099</v>
       </c>
       <c r="AC45" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.348</v>
       </c>
       <c r="AD45" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.110
 (0.099)</v>
       </c>
-    </row>
-    <row r="46" spans="1:30">
+      <c r="AE45" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -7784,32 +8100,36 @@
         <v>15</v>
       </c>
       <c r="Y46" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>all_no_live_liner_I(job7V*100)</v>
       </c>
       <c r="Z46" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>569983</v>
       </c>
       <c r="AA46" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.111</v>
       </c>
       <c r="AB46" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.099</v>
       </c>
       <c r="AC46" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.358</v>
       </c>
       <c r="AD46" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.111
 (0.099)</v>
       </c>
-    </row>
-    <row r="47" spans="1:30">
+      <c r="AE46" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="47" spans="1:31">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -7868,32 +8188,36 @@
         <v>14</v>
       </c>
       <c r="Y47" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>all_ols_liner_age_father</v>
       </c>
       <c r="Z47" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>559098</v>
       </c>
       <c r="AA47" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.128</v>
       </c>
       <c r="AB47" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.024</v>
       </c>
       <c r="AC47" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>NA</v>
       </c>
       <c r="AD47" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.128
 (0.024)</v>
       </c>
-    </row>
-    <row r="48" spans="1:30">
+      <c r="AE47" t="str">
+        <f t="shared" si="6"/>
+        <v>559098</v>
+      </c>
+    </row>
+    <row r="48" spans="1:31">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -7952,32 +8276,36 @@
         <v>14</v>
       </c>
       <c r="Y48" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>all_ols_liner_age_mother</v>
       </c>
       <c r="Z48" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>569981</v>
       </c>
       <c r="AA48" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.113</v>
       </c>
       <c r="AB48" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.021</v>
       </c>
       <c r="AC48" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>NA</v>
       </c>
       <c r="AD48" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.113
 (0.021)</v>
       </c>
-    </row>
-    <row r="49" spans="1:30">
+      <c r="AE48" t="str">
+        <f t="shared" si="6"/>
+        <v>569981</v>
+      </c>
+    </row>
+    <row r="49" spans="1:31">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -8036,32 +8364,36 @@
         <v>14</v>
       </c>
       <c r="Y49" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>all_ols_liner_I(no_legitimate*100)</v>
       </c>
       <c r="Z49" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>569983</v>
       </c>
       <c r="AA49" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.056</v>
       </c>
       <c r="AB49" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.072</v>
       </c>
       <c r="AC49" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>NA</v>
       </c>
       <c r="AD49" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.056
 (0.072)</v>
       </c>
-    </row>
-    <row r="50" spans="1:30">
+      <c r="AE49" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="50" spans="1:31">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -8120,33 +8452,37 @@
         <v>14</v>
       </c>
       <c r="Y50" s="1" t="str">
-        <f t="shared" ref="Y50:Y73" si="12">N50</f>
+        <f t="shared" ref="Y50:Y73" si="13">N50</f>
         <v>all_ols_liner_gram</v>
       </c>
       <c r="Z50" s="1">
-        <f t="shared" ref="Z50:Z73" si="13">ROUND(I50, 3)</f>
+        <f t="shared" ref="Z50:Z73" si="14">ROUND(I50, 3)</f>
         <v>569535</v>
       </c>
       <c r="AA50" s="1" t="str">
-        <f t="shared" ref="AA50:AA73" si="14">TEXT(K50,"0.000")</f>
+        <f t="shared" ref="AA50:AA73" si="15">TEXT(K50,"0.000")</f>
         <v>2.382</v>
       </c>
       <c r="AB50" s="1" t="str">
-        <f t="shared" ref="AB50:AB73" si="15">TEXT(L50,"0.000")</f>
+        <f t="shared" ref="AB50:AB73" si="16">TEXT(L50,"0.000")</f>
         <v>1.905</v>
       </c>
       <c r="AC50" s="1" t="str">
-        <f t="shared" ref="AC50:AC73" si="16">TEXT(R50,"0.000")</f>
+        <f t="shared" ref="AC50:AC73" si="17">TEXT(R50,"0.000")</f>
         <v>NA</v>
       </c>
       <c r="AD50" t="str">
-        <f t="shared" ref="AD50:AD73" si="17">CONCATENATE(AA50,"
+        <f t="shared" ref="AD50:AD73" si="18">CONCATENATE(AA50,"
 (",AB50,")")</f>
         <v>2.382
 (1.905)</v>
       </c>
-    </row>
-    <row r="51" spans="1:30">
+      <c r="AE50" t="str">
+        <f t="shared" si="6"/>
+        <v>569535</v>
+      </c>
+    </row>
+    <row r="51" spans="1:31">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -8205,32 +8541,36 @@
         <v>14</v>
       </c>
       <c r="Y51" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>all_ols_liner_pregnant_week</v>
       </c>
       <c r="Z51" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>569784</v>
       </c>
       <c r="AA51" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.002</v>
       </c>
       <c r="AB51" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.009</v>
       </c>
       <c r="AC51" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="AD51" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-0.002
 (0.009)</v>
       </c>
-    </row>
-    <row r="52" spans="1:30">
+      <c r="AE51" t="str">
+        <f t="shared" si="6"/>
+        <v>569784</v>
+      </c>
+    </row>
+    <row r="52" spans="1:31">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -8289,32 +8629,36 @@
         <v>14</v>
       </c>
       <c r="Y52" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>all_ols_liner_I(single_womb*100)</v>
       </c>
       <c r="Z52" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>569983</v>
       </c>
       <c r="AA52" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.076</v>
       </c>
       <c r="AB52" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.082</v>
       </c>
       <c r="AC52" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="AD52" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-0.076
 (0.082)</v>
       </c>
-    </row>
-    <row r="53" spans="1:30">
+      <c r="AE52" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="53" spans="1:31">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -8373,32 +8717,36 @@
         <v>14</v>
       </c>
       <c r="Y53" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>all_ols_liner_I(firstborn*100)</v>
       </c>
       <c r="Z53" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>569983</v>
       </c>
       <c r="AA53" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.973</v>
       </c>
       <c r="AB53" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.260</v>
       </c>
       <c r="AC53" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="AD53" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-0.973
 (0.260)</v>
       </c>
-    </row>
-    <row r="54" spans="1:30">
+      <c r="AE53" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="54" spans="1:31">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -8457,32 +8805,36 @@
         <v>14</v>
       </c>
       <c r="Y54" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>all_ols_liner_I(girl*100)</v>
       </c>
       <c r="Z54" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>569983</v>
       </c>
       <c r="AA54" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.324</v>
       </c>
       <c r="AB54" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.241</v>
       </c>
       <c r="AC54" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="AD54" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-0.324
 (0.241)</v>
       </c>
-    </row>
-    <row r="55" spans="1:30">
+      <c r="AE54" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="55" spans="1:31">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -8541,32 +8893,36 @@
         <v>14</v>
       </c>
       <c r="Y55" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>all_ols_liner_I(job1*100)</v>
       </c>
       <c r="Z55" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>569983</v>
       </c>
       <c r="AA55" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.001</v>
       </c>
       <c r="AB55" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.039</v>
       </c>
       <c r="AC55" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="AD55" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-0.001
 (0.039)</v>
       </c>
-    </row>
-    <row r="56" spans="1:30">
+      <c r="AE55" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="56" spans="1:31">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -8625,32 +8981,36 @@
         <v>14</v>
       </c>
       <c r="Y56" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>all_ols_liner_I(job2*100)</v>
       </c>
       <c r="Z56" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>569983</v>
       </c>
       <c r="AA56" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.176</v>
       </c>
       <c r="AB56" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.106</v>
       </c>
       <c r="AC56" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="AD56" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-0.176
 (0.106)</v>
       </c>
-    </row>
-    <row r="57" spans="1:30">
+      <c r="AE56" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="57" spans="1:31">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -8709,32 +9069,36 @@
         <v>14</v>
       </c>
       <c r="Y57" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>all_ols_liner_I(job3*100)</v>
       </c>
       <c r="Z57" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>569983</v>
       </c>
       <c r="AA57" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.058</v>
       </c>
       <c r="AB57" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.235</v>
       </c>
       <c r="AC57" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="AD57" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-0.058
 (0.235)</v>
       </c>
-    </row>
-    <row r="58" spans="1:30">
+      <c r="AE57" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="58" spans="1:31">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -8793,32 +9157,36 @@
         <v>14</v>
       </c>
       <c r="Y58" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>all_ols_liner_I(job4*100)</v>
       </c>
       <c r="Z58" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>569983</v>
       </c>
       <c r="AA58" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.209</v>
       </c>
       <c r="AB58" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.180</v>
       </c>
       <c r="AC58" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="AD58" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-0.209
 (0.180)</v>
       </c>
-    </row>
-    <row r="59" spans="1:30">
+      <c r="AE58" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="59" spans="1:31">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -8877,32 +9245,36 @@
         <v>14</v>
       </c>
       <c r="Y59" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>all_ols_liner_I(job5*100)</v>
       </c>
       <c r="Z59" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>569983</v>
       </c>
       <c r="AA59" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.506</v>
       </c>
       <c r="AB59" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.122</v>
       </c>
       <c r="AC59" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="AD59" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.506
 (0.122)</v>
       </c>
-    </row>
-    <row r="60" spans="1:30">
+      <c r="AE59" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="60" spans="1:31">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -8961,32 +9333,36 @@
         <v>14</v>
       </c>
       <c r="Y60" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>all_ols_liner_I(job6*100)</v>
       </c>
       <c r="Z60" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>569983</v>
       </c>
       <c r="AA60" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.147</v>
       </c>
       <c r="AB60" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.050</v>
       </c>
       <c r="AC60" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="AD60" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-0.147
 (0.050)</v>
       </c>
-    </row>
-    <row r="61" spans="1:30">
+      <c r="AE60" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="61" spans="1:31">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -9045,32 +9421,36 @@
         <v>14</v>
       </c>
       <c r="Y61" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>all_ols_liner_I(job7V*100)</v>
       </c>
       <c r="Z61" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>569983</v>
       </c>
       <c r="AA61" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.084</v>
       </c>
       <c r="AB61" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.187</v>
       </c>
       <c r="AC61" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="AD61" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.084
 (0.187)</v>
       </c>
-    </row>
-    <row r="62" spans="1:30">
+      <c r="AE61" t="str">
+        <f t="shared" si="6"/>
+        <v>569983</v>
+      </c>
+    </row>
+    <row r="62" spans="1:31">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -9129,32 +9509,36 @@
         <v>14</v>
       </c>
       <c r="Y62" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>all_ols_I(is_white_work_father*100)</v>
       </c>
       <c r="Z62" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>176634</v>
       </c>
       <c r="AA62" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3.706</v>
       </c>
       <c r="AB62" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.758</v>
       </c>
       <c r="AC62" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="AD62" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>3.706
 (0.758)</v>
       </c>
-    </row>
-    <row r="63" spans="1:30">
+      <c r="AE62" t="str">
+        <f t="shared" si="6"/>
+        <v>176634</v>
+      </c>
+    </row>
+    <row r="63" spans="1:31">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -9213,32 +9597,36 @@
         <v>14</v>
       </c>
       <c r="Y63" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>all_ols_liner_I(is_white_work_father*100)</v>
       </c>
       <c r="Z63" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>176634</v>
       </c>
       <c r="AA63" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3.705</v>
       </c>
       <c r="AB63" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.758</v>
       </c>
       <c r="AC63" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="AD63" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>3.705
 (0.758)</v>
       </c>
-    </row>
-    <row r="64" spans="1:30">
+      <c r="AE63" t="str">
+        <f t="shared" si="6"/>
+        <v>176634</v>
+      </c>
+    </row>
+    <row r="64" spans="1:31">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -9297,32 +9685,36 @@
         <v>14</v>
       </c>
       <c r="Y64" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>all_ols_I(is_white_work_mother*100)</v>
       </c>
       <c r="Z64" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>176634</v>
       </c>
       <c r="AA64" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.077</v>
       </c>
       <c r="AB64" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.524</v>
       </c>
       <c r="AC64" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="AD64" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.077
 (0.524)</v>
       </c>
-    </row>
-    <row r="65" spans="1:30">
+      <c r="AE64" t="str">
+        <f t="shared" si="6"/>
+        <v>176634</v>
+      </c>
+    </row>
+    <row r="65" spans="1:31">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -9381,32 +9773,36 @@
         <v>14</v>
       </c>
       <c r="Y65" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>all_ols_liner_I(is_white_work_mother*100)</v>
       </c>
       <c r="Z65" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>176634</v>
       </c>
       <c r="AA65" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.077</v>
       </c>
       <c r="AB65" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.524</v>
       </c>
       <c r="AC65" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="AD65" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.077
 (0.524)</v>
       </c>
-    </row>
-    <row r="66" spans="1:30">
+      <c r="AE65" t="str">
+        <f t="shared" si="6"/>
+        <v>176634</v>
+      </c>
+    </row>
+    <row r="66" spans="1:31">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -9465,32 +9861,36 @@
         <v>14</v>
       </c>
       <c r="Y66" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>all_ols_I(no_job_father*100)</v>
       </c>
       <c r="Z66" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>176634</v>
       </c>
       <c r="AA66" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.058</v>
       </c>
       <c r="AB66" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.079</v>
       </c>
       <c r="AC66" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="AD66" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.058
 (0.079)</v>
       </c>
-    </row>
-    <row r="67" spans="1:30">
+      <c r="AE66" t="str">
+        <f t="shared" si="6"/>
+        <v>176634</v>
+      </c>
+    </row>
+    <row r="67" spans="1:31">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -9549,32 +9949,36 @@
         <v>14</v>
       </c>
       <c r="Y67" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>all_ols_liner_I(no_job_father*100)</v>
       </c>
       <c r="Z67" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>176634</v>
       </c>
       <c r="AA67" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.058</v>
       </c>
       <c r="AB67" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.079</v>
       </c>
       <c r="AC67" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="AD67" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.058
 (0.079)</v>
       </c>
-    </row>
-    <row r="68" spans="1:30">
+      <c r="AE67" t="str">
+        <f t="shared" ref="AE67:AE77" si="19">TEXT(I67,"0")</f>
+        <v>176634</v>
+      </c>
+    </row>
+    <row r="68" spans="1:31">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -9633,32 +10037,36 @@
         <v>14</v>
       </c>
       <c r="Y68" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>all_ols_I(no_job_mother*100)</v>
       </c>
       <c r="Z68" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>176634</v>
       </c>
       <c r="AA68" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3.303</v>
       </c>
       <c r="AB68" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.625</v>
       </c>
       <c r="AC68" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="AD68" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>3.303
 (0.625)</v>
       </c>
-    </row>
-    <row r="69" spans="1:30">
+      <c r="AE68" t="str">
+        <f t="shared" si="19"/>
+        <v>176634</v>
+      </c>
+    </row>
+    <row r="69" spans="1:31">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -9717,261 +10125,297 @@
         <v>14</v>
       </c>
       <c r="Y69" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>all_ols_liner_I(no_job_mother*100)</v>
       </c>
       <c r="Z69" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>176634</v>
       </c>
       <c r="AA69" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3.302</v>
       </c>
       <c r="AB69" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.624</v>
       </c>
       <c r="AC69" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="AD69" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>3.302
 (0.624)</v>
       </c>
-    </row>
-    <row r="70" spans="1:30">
+      <c r="AE69" t="str">
+        <f t="shared" si="19"/>
+        <v>176634</v>
+      </c>
+    </row>
+    <row r="70" spans="1:31">
       <c r="Y70" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="Z70" s="1">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
+      <c r="Z70" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
       <c r="AA70" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.000</v>
       </c>
       <c r="AB70" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.000</v>
       </c>
       <c r="AC70" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.000</v>
       </c>
       <c r="AD70" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.000
 (0.000)</v>
       </c>
-    </row>
-    <row r="71" spans="1:30">
+      <c r="AE70" t="str">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:31">
       <c r="Y71" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="Z71" s="1">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
+      <c r="Z71" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
       <c r="AA71" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.000</v>
       </c>
       <c r="AB71" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.000</v>
       </c>
       <c r="AC71" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.000</v>
       </c>
       <c r="AD71" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.000
 (0.000)</v>
       </c>
-    </row>
-    <row r="72" spans="1:30">
+      <c r="AE71" t="str">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:31">
       <c r="Y72" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="Z72" s="1">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
+      <c r="Z72" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
       <c r="AA72" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.000</v>
       </c>
       <c r="AB72" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.000</v>
       </c>
       <c r="AC72" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.000</v>
       </c>
       <c r="AD72" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.000
 (0.000)</v>
       </c>
-    </row>
-    <row r="73" spans="1:30">
+      <c r="AE72" t="str">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:31">
       <c r="Y73" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="Z73" s="1">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
+      <c r="Z73" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
       <c r="AA73" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.000</v>
       </c>
       <c r="AB73" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.000</v>
       </c>
       <c r="AC73" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.000</v>
       </c>
       <c r="AD73" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.000
 (0.000)</v>
       </c>
-    </row>
-    <row r="74" spans="1:30">
+      <c r="AE73" t="str">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:31">
       <c r="Y74" s="1">
-        <f t="shared" ref="Y74:Y77" si="18">N74</f>
+        <f t="shared" ref="Y74:Y77" si="20">N74</f>
         <v>0</v>
       </c>
       <c r="Z74" s="1">
-        <f t="shared" ref="Z74:Z77" si="19">ROUND(I74, 3)</f>
+        <f t="shared" ref="Z74:Z77" si="21">ROUND(I74, 3)</f>
         <v>0</v>
       </c>
       <c r="AA74" s="1" t="str">
-        <f t="shared" ref="AA74:AA77" si="20">TEXT(K74,"0.000")</f>
+        <f t="shared" ref="AA74:AA77" si="22">TEXT(K74,"0.000")</f>
         <v>0.000</v>
       </c>
       <c r="AB74" s="1" t="str">
-        <f t="shared" ref="AB74:AB77" si="21">TEXT(L74,"0.000")</f>
+        <f t="shared" ref="AB74:AB77" si="23">TEXT(L74,"0.000")</f>
         <v>0.000</v>
       </c>
       <c r="AC74" s="1" t="str">
-        <f t="shared" ref="AC74:AC77" si="22">TEXT(R74,"0.000")</f>
+        <f t="shared" ref="AC74:AC77" si="24">TEXT(R74,"0.000")</f>
         <v>0.000</v>
       </c>
       <c r="AD74" t="str">
-        <f t="shared" ref="AD74:AD77" si="23">CONCATENATE(AA74,"
+        <f t="shared" ref="AD74:AD77" si="25">CONCATENATE(AA74,"
 (",AB74,")")</f>
         <v>0.000
 (0.000)</v>
       </c>
-    </row>
-    <row r="75" spans="1:30">
-      <c r="Y75" s="1">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="Z75" s="1">
+      <c r="AE74" t="str">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
+    </row>
+    <row r="75" spans="1:31">
+      <c r="Y75" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="Z75" s="1">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
       <c r="AA75" s="1" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.000</v>
       </c>
       <c r="AB75" s="1" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0.000</v>
       </c>
       <c r="AC75" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0.000</v>
       </c>
       <c r="AD75" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.000
 (0.000)</v>
       </c>
-    </row>
-    <row r="76" spans="1:30">
-      <c r="Y76" s="1">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="Z76" s="1">
+      <c r="AE75" t="str">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
+    </row>
+    <row r="76" spans="1:31">
+      <c r="Y76" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="Z76" s="1">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
       <c r="AA76" s="1" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.000</v>
       </c>
       <c r="AB76" s="1" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0.000</v>
       </c>
       <c r="AC76" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0.000</v>
       </c>
       <c r="AD76" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.000
 (0.000)</v>
       </c>
-    </row>
-    <row r="77" spans="1:30">
-      <c r="Y77" s="1">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="Z77" s="1">
+      <c r="AE76" t="str">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
+    </row>
+    <row r="77" spans="1:31">
+      <c r="Y77" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="Z77" s="1">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
       <c r="AA77" s="1" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.000</v>
       </c>
       <c r="AB77" s="1" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0.000</v>
       </c>
       <c r="AC77" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0.000</v>
       </c>
       <c r="AD77" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.000
 (0.000)</v>
       </c>
-    </row>
-    <row r="78" spans="1:30">
+      <c r="AE77" t="str">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:31">
       <c r="Y78" s="1"/>
       <c r="Z78" s="1"/>
       <c r="AA78" s="1"/>
       <c r="AB78" s="1"/>
     </row>
-    <row r="79" spans="1:30">
+    <row r="79" spans="1:31">
       <c r="Y79" s="1"/>
       <c r="Z79" s="1"/>
       <c r="AA79" s="1"/>
       <c r="AB79" s="1"/>
     </row>
-    <row r="80" spans="1:30">
+    <row r="80" spans="1:31">
       <c r="Y80" s="1"/>
       <c r="Z80" s="1"/>
       <c r="AA80" s="1"/>

</xml_diff>